<commit_message>
Revamped processing, moved most scripts into "AeolianFieldworkAnalysis"
</commit_message>
<xml_diff>
--- a/Metadata/InstrumentMetadata_OceanoCalibration.xlsx
+++ b/Metadata/InstrumentMetadata_OceanoCalibration.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-260" yWindow="0" windowWidth="19660" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="19340" yWindow="4180" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="61">
   <si>
     <t>Site</t>
   </si>
@@ -143,6 +143,69 @@
   <si>
     <t>C2</t>
   </si>
+  <si>
+    <t>InstrumentID</t>
+  </si>
+  <si>
+    <t>J3301</t>
+  </si>
+  <si>
+    <t>J3306</t>
+  </si>
+  <si>
+    <t>J3311</t>
+  </si>
+  <si>
+    <t>J8607</t>
+  </si>
+  <si>
+    <t>9284</t>
+  </si>
+  <si>
+    <t>9290</t>
+  </si>
+  <si>
+    <t>9281</t>
+  </si>
+  <si>
+    <t>9278</t>
+  </si>
+  <si>
+    <t>9287</t>
+  </si>
+  <si>
+    <t>0370</t>
+  </si>
+  <si>
+    <t>0367</t>
+  </si>
+  <si>
+    <t>0377</t>
+  </si>
+  <si>
+    <t>0369</t>
+  </si>
+  <si>
+    <t>0274</t>
+  </si>
+  <si>
+    <t>1099</t>
+  </si>
+  <si>
+    <t>02379</t>
+  </si>
+  <si>
+    <t>02309</t>
+  </si>
+  <si>
+    <t>02380</t>
+  </si>
+  <si>
+    <t>02354</t>
+  </si>
+  <si>
+    <t>43282163</t>
+  </si>
 </sst>
 </file>
 
@@ -151,7 +214,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss.00"/>
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -220,7 +283,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1337">
+  <cellStyleXfs count="1381">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1558,8 +1621,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1567,10 +1674,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1337">
+  <cellStyles count="1381">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2239,6 +2347,28 @@
     <cellStyle name="Followed Hyperlink" xfId="1332" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1334" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1380" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2907,6 +3037,28 @@
     <cellStyle name="Hyperlink" xfId="1331" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1333" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1379" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3236,12 +3388,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3263,7 +3415,7 @@
     <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1">
+    <row r="1" spans="1:15" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3306,25 +3458,28 @@
       <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="5">
-        <v>42160</v>
+        <v>42162</v>
       </c>
       <c r="C2" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D2" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="G2" s="4">
         <v>1.49</v>
@@ -3350,8 +3505,11 @@
       <c r="N2" s="4">
         <v>0</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="4" t="s">
         <v>38</v>
       </c>
@@ -3368,7 +3526,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="4">
         <v>1.49</v>
@@ -3386,7 +3544,7 @@
         <v>0.4</v>
       </c>
       <c r="L3" s="4">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="M3" s="4">
         <v>0</v>
@@ -3394,25 +3552,28 @@
       <c r="N3" s="4">
         <v>0</v>
       </c>
+      <c r="O3" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="5">
-        <v>42160</v>
+        <v>42161</v>
       </c>
       <c r="C4" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D4" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4" s="4">
         <v>1.49</v>
@@ -3430,7 +3591,7 @@
         <v>0.4</v>
       </c>
       <c r="L4" s="4">
-        <v>-3.6</v>
+        <v>-2</v>
       </c>
       <c r="M4" s="4">
         <v>0</v>
@@ -3438,8 +3599,11 @@
       <c r="N4" s="4">
         <v>0</v>
       </c>
+      <c r="O4" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="4" t="s">
         <v>38</v>
       </c>
@@ -3453,10 +3617,10 @@
         <v>0.73472222222222217</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G5" s="4">
         <v>1.49</v>
@@ -3471,10 +3635,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="4">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="L5" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M5" s="4">
         <v>0</v>
@@ -3482,25 +3646,28 @@
       <c r="N5" s="4">
         <v>0</v>
       </c>
+      <c r="O5" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="5">
-        <v>42160</v>
+        <v>42161</v>
       </c>
       <c r="C6" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D6" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G6" s="4">
         <v>1.49</v>
@@ -3515,10 +3682,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="L6" s="4">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="M6" s="4">
         <v>0</v>
@@ -3526,25 +3693,28 @@
       <c r="N6" s="4">
         <v>0</v>
       </c>
+      <c r="O6" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="5">
-        <v>42160</v>
+        <v>42162</v>
       </c>
       <c r="C7" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D7" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="G7" s="4">
         <v>1.49</v>
@@ -3559,10 +3729,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="L7" s="4">
-        <v>4.4000000000000004</v>
+        <v>-3.6</v>
       </c>
       <c r="M7" s="4">
         <v>0</v>
@@ -3570,8 +3740,11 @@
       <c r="N7" s="4">
         <v>0</v>
       </c>
+      <c r="O7" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="4" t="s">
         <v>38</v>
       </c>
@@ -3585,10 +3758,10 @@
         <v>0.73472222222222217</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G8" s="4">
         <v>1.49</v>
@@ -3603,10 +3776,10 @@
         <v>0</v>
       </c>
       <c r="K8" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="L8" s="4">
-        <v>-4.4000000000000004</v>
+        <v>-3.6</v>
       </c>
       <c r="M8" s="4">
         <v>0</v>
@@ -3614,25 +3787,28 @@
       <c r="N8" s="4">
         <v>0</v>
       </c>
+      <c r="O8" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="5">
-        <v>42160</v>
+        <v>42161</v>
       </c>
       <c r="C9" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D9" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="G9" s="4">
         <v>1.49</v>
@@ -3647,10 +3823,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="L9" s="4">
-        <v>-1.2</v>
+        <v>-3.6</v>
       </c>
       <c r="M9" s="4">
         <v>0</v>
@@ -3658,25 +3834,28 @@
       <c r="N9" s="4">
         <v>0</v>
       </c>
+      <c r="O9" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="5">
-        <v>42160</v>
+        <v>42162</v>
       </c>
       <c r="C10" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D10" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G10" s="4">
         <v>1.49</v>
@@ -3691,10 +3870,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="L10" s="4">
-        <v>-2.8</v>
+        <v>2</v>
       </c>
       <c r="M10" s="4">
         <v>0</v>
@@ -3702,8 +3881,11 @@
       <c r="N10" s="4">
         <v>0</v>
       </c>
+      <c r="O10" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -3717,16 +3899,16 @@
         <v>0.73472222222222217</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G11" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H11" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I11" s="4">
         <v>0.01</v>
@@ -3735,7 +3917,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L11" s="4">
         <v>5.2</v>
@@ -3746,31 +3928,34 @@
       <c r="N11" s="4">
         <v>0</v>
       </c>
+      <c r="O11" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="5">
-        <v>42160</v>
+        <v>42161</v>
       </c>
       <c r="C12" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="D12" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.63055555555555554</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G12" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H12" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I12" s="4">
         <v>0.01</v>
@@ -3779,10 +3964,10 @@
         <v>0</v>
       </c>
       <c r="K12" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L12" s="4">
-        <v>2.8</v>
+        <v>5.2</v>
       </c>
       <c r="M12" s="4">
         <v>0</v>
@@ -3790,31 +3975,34 @@
       <c r="N12" s="4">
         <v>0</v>
       </c>
+      <c r="O12" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="5">
-        <v>42160</v>
+        <v>42162</v>
       </c>
       <c r="C13" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D13" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G13" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H13" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I13" s="4">
         <v>0.01</v>
@@ -3823,10 +4011,10 @@
         <v>0</v>
       </c>
       <c r="K13" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L13" s="4">
-        <v>-0.4</v>
+        <v>0.4</v>
       </c>
       <c r="M13" s="4">
         <v>0</v>
@@ -3834,8 +4022,11 @@
       <c r="N13" s="4">
         <v>0</v>
       </c>
+      <c r="O13" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" s="4" t="s">
         <v>38</v>
       </c>
@@ -3849,16 +4040,16 @@
         <v>0.73472222222222217</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G14" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H14" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I14" s="4">
         <v>0.01</v>
@@ -3867,10 +4058,10 @@
         <v>0</v>
       </c>
       <c r="K14" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L14" s="4">
-        <v>-5.2</v>
+        <v>2.8</v>
       </c>
       <c r="M14" s="4">
         <v>0</v>
@@ -3878,31 +4069,34 @@
       <c r="N14" s="4">
         <v>0</v>
       </c>
+      <c r="O14" s="9" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="5">
-        <v>42160</v>
+        <v>42161</v>
       </c>
       <c r="C15" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="D15" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.63055555555555554</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G15" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H15" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I15" s="4">
         <v>0.01</v>
@@ -3911,10 +4105,10 @@
         <v>0</v>
       </c>
       <c r="K15" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L15" s="4">
-        <v>0.4</v>
+        <v>2.8</v>
       </c>
       <c r="M15" s="4">
         <v>0</v>
@@ -3922,25 +4116,28 @@
       <c r="N15" s="4">
         <v>0</v>
       </c>
+      <c r="O15" s="9" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="5">
-        <v>42160</v>
+        <v>42162</v>
       </c>
       <c r="C16" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D16" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G16" s="4">
         <v>1.95</v>
@@ -3958,7 +4155,7 @@
         <v>0.75</v>
       </c>
       <c r="L16" s="4">
-        <v>5.2</v>
+        <v>-0.4</v>
       </c>
       <c r="M16" s="4">
         <v>0</v>
@@ -3966,8 +4163,11 @@
       <c r="N16" s="4">
         <v>0</v>
       </c>
+      <c r="O16" s="9" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -3984,7 +4184,7 @@
         <v>27</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G17" s="4">
         <v>1.95</v>
@@ -4002,7 +4202,7 @@
         <v>0.75</v>
       </c>
       <c r="L17" s="4">
-        <v>2.8</v>
+        <v>-2.8</v>
       </c>
       <c r="M17" s="4">
         <v>0</v>
@@ -4010,19 +4210,22 @@
       <c r="N17" s="4">
         <v>0</v>
       </c>
+      <c r="O17" s="9" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="5">
-        <v>42160</v>
+        <v>42161</v>
       </c>
       <c r="C18" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="D18" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.63055555555555554</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>27</v>
@@ -4054,25 +4257,28 @@
       <c r="N18" s="4">
         <v>0</v>
       </c>
+      <c r="O18" s="9" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="5">
-        <v>42160</v>
+        <v>42162</v>
       </c>
       <c r="C19" s="8">
-        <v>0.71388888888888891</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D19" s="8">
-        <v>0.73472222222222217</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G19" s="4">
         <v>1.95</v>
@@ -4090,7 +4296,7 @@
         <v>0.75</v>
       </c>
       <c r="L19" s="4">
-        <v>-0.4</v>
+        <v>2.8</v>
       </c>
       <c r="M19" s="4">
         <v>0</v>
@@ -4098,8 +4304,11 @@
       <c r="N19" s="4">
         <v>0</v>
       </c>
+      <c r="O19" s="9" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
@@ -4116,7 +4325,7 @@
         <v>27</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G20" s="4">
         <v>1.95</v>
@@ -4134,7 +4343,7 @@
         <v>0.75</v>
       </c>
       <c r="L20" s="4">
-        <v>0.4</v>
+        <v>-0.4</v>
       </c>
       <c r="M20" s="4">
         <v>0</v>
@@ -4142,8 +4351,11 @@
       <c r="N20" s="4">
         <v>0</v>
       </c>
+      <c r="O20" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15">
       <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
@@ -4151,22 +4363,22 @@
         <v>42161</v>
       </c>
       <c r="C21" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="D21" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.63055555555555554</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G21" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H21" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I21" s="4">
         <v>0.01</v>
@@ -4175,10 +4387,10 @@
         <v>0</v>
       </c>
       <c r="K21" s="4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L21" s="4">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
       <c r="M21" s="4">
         <v>0</v>
@@ -4186,31 +4398,34 @@
       <c r="N21" s="4">
         <v>0</v>
       </c>
+      <c r="O21" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="5">
-        <v>42161</v>
+        <v>42162</v>
       </c>
       <c r="C22" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D22" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G22" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H22" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I22" s="4">
         <v>0.01</v>
@@ -4219,10 +4434,10 @@
         <v>0</v>
       </c>
       <c r="K22" s="4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L22" s="4">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="M22" s="4">
         <v>0</v>
@@ -4230,31 +4445,34 @@
       <c r="N22" s="4">
         <v>0</v>
       </c>
+      <c r="O22" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="5">
-        <v>42161</v>
+        <v>42160</v>
       </c>
       <c r="C23" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D23" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G23" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H23" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I23" s="4">
         <v>0.01</v>
@@ -4263,19 +4481,22 @@
         <v>0</v>
       </c>
       <c r="K23" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="L23" s="4">
         <v>0.4</v>
       </c>
-      <c r="L23" s="4">
-        <v>-3.6</v>
-      </c>
       <c r="M23" s="4">
         <v>0</v>
       </c>
       <c r="N23" s="4">
         <v>0</v>
       </c>
+      <c r="O23" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15">
       <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
@@ -4283,22 +4504,22 @@
         <v>42161</v>
       </c>
       <c r="C24" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="D24" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.63055555555555554</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="G24" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H24" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I24" s="4">
         <v>0.01</v>
@@ -4307,10 +4528,10 @@
         <v>0</v>
       </c>
       <c r="K24" s="4">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="L24" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="M24" s="4">
         <v>0</v>
@@ -4318,31 +4539,34 @@
       <c r="N24" s="4">
         <v>0</v>
       </c>
+      <c r="O24" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15">
       <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="5">
-        <v>42161</v>
+        <v>42162</v>
       </c>
       <c r="C25" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D25" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G25" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="H25" s="4">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="I25" s="4">
         <v>0.01</v>
@@ -4351,10 +4575,10 @@
         <v>0</v>
       </c>
       <c r="K25" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L25" s="4">
-        <v>1.2</v>
+        <v>-2.8</v>
       </c>
       <c r="M25" s="4">
         <v>0</v>
@@ -4362,25 +4586,28 @@
       <c r="N25" s="4">
         <v>0</v>
       </c>
+      <c r="O25" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:15">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="5">
-        <v>42161</v>
+        <v>42160</v>
       </c>
       <c r="C26" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D26" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G26" s="4">
         <v>1.49</v>
@@ -4398,7 +4625,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="4">
-        <v>4.4000000000000004</v>
+        <v>-2.8</v>
       </c>
       <c r="M26" s="4">
         <v>0</v>
@@ -4406,8 +4633,11 @@
       <c r="N26" s="4">
         <v>0</v>
       </c>
+      <c r="O26" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:15">
       <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
@@ -4421,10 +4651,10 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G27" s="4">
         <v>1.49</v>
@@ -4442,7 +4672,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="4">
-        <v>-4.4000000000000004</v>
+        <v>-2.8</v>
       </c>
       <c r="M27" s="4">
         <v>0</v>
@@ -4450,25 +4680,28 @@
       <c r="N27" s="4">
         <v>0</v>
       </c>
+      <c r="O27" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:15">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="5">
-        <v>42161</v>
+        <v>42162</v>
       </c>
       <c r="C28" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D28" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G28" s="4">
         <v>1.49</v>
@@ -4486,7 +4719,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="4">
-        <v>-1.2</v>
+        <v>2.8</v>
       </c>
       <c r="M28" s="4">
         <v>0</v>
@@ -4494,25 +4727,28 @@
       <c r="N28" s="4">
         <v>0</v>
       </c>
+      <c r="O28" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:15">
       <c r="A29" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="5">
-        <v>42161</v>
+        <v>42160</v>
       </c>
       <c r="C29" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D29" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G29" s="4">
         <v>1.49</v>
@@ -4530,7 +4766,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="4">
-        <v>-2.8</v>
+        <v>5.2</v>
       </c>
       <c r="M29" s="4">
         <v>0</v>
@@ -4538,8 +4774,11 @@
       <c r="N29" s="4">
         <v>0</v>
       </c>
+      <c r="O29" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:15">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
@@ -4582,25 +4821,28 @@
       <c r="N30" s="4">
         <v>0</v>
       </c>
+      <c r="O30" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:15">
       <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B31" s="5">
-        <v>42161</v>
+        <v>42162</v>
       </c>
       <c r="C31" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D31" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G31" s="4">
         <v>1.49</v>
@@ -4618,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="4">
-        <v>2.8</v>
+        <v>-0.4</v>
       </c>
       <c r="M31" s="4">
         <v>0</v>
@@ -4626,25 +4868,28 @@
       <c r="N31" s="4">
         <v>0</v>
       </c>
+      <c r="O31" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:15">
       <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="5">
-        <v>42161</v>
+        <v>42160</v>
       </c>
       <c r="C32" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D32" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G32" s="4">
         <v>1.49</v>
@@ -4662,7 +4907,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="4">
-        <v>-0.4</v>
+        <v>2.8</v>
       </c>
       <c r="M32" s="4">
         <v>0</v>
@@ -4670,8 +4915,11 @@
       <c r="N32" s="4">
         <v>0</v>
       </c>
+      <c r="O32" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:15">
       <c r="A33" s="4" t="s">
         <v>38</v>
       </c>
@@ -4688,7 +4936,7 @@
         <v>20</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G33" s="4">
         <v>1.49</v>
@@ -4706,7 +4954,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="4">
-        <v>-5.2</v>
+        <v>2.8</v>
       </c>
       <c r="M33" s="4">
         <v>0</v>
@@ -4714,25 +4962,28 @@
       <c r="N33" s="4">
         <v>0</v>
       </c>
+      <c r="O33" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:15">
       <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="5">
-        <v>42161</v>
+        <v>42162</v>
       </c>
       <c r="C34" s="8">
-        <v>0.65277777777777779</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D34" s="8">
-        <v>0.77777777777777779</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G34" s="4">
         <v>1.49</v>
@@ -4750,7 +5001,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="4">
-        <v>0.4</v>
+        <v>-2.8</v>
       </c>
       <c r="M34" s="4">
         <v>0</v>
@@ -4758,31 +5009,34 @@
       <c r="N34" s="4">
         <v>0</v>
       </c>
+      <c r="O34" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:15">
       <c r="A35" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="5">
-        <v>42161</v>
+        <v>42160</v>
       </c>
       <c r="C35" s="8">
-        <v>0.43402777777777773</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D35" s="8">
-        <v>0.63055555555555554</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G35" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H35" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I35" s="4">
         <v>0.01</v>
@@ -4791,10 +5045,10 @@
         <v>0</v>
       </c>
       <c r="K35" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L35" s="4">
-        <v>5.2</v>
+        <v>-0.4</v>
       </c>
       <c r="M35" s="4">
         <v>0</v>
@@ -4802,8 +5056,11 @@
       <c r="N35" s="4">
         <v>0</v>
       </c>
+      <c r="O35" s="9" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:15">
       <c r="A36" s="4" t="s">
         <v>38</v>
       </c>
@@ -4811,22 +5068,22 @@
         <v>42161</v>
       </c>
       <c r="C36" s="8">
-        <v>0.43402777777777773</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D36" s="8">
-        <v>0.63055555555555554</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G36" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H36" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I36" s="4">
         <v>0.01</v>
@@ -4835,10 +5092,10 @@
         <v>0</v>
       </c>
       <c r="K36" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L36" s="4">
-        <v>2.8</v>
+        <v>-0.4</v>
       </c>
       <c r="M36" s="4">
         <v>0</v>
@@ -4846,31 +5103,34 @@
       <c r="N36" s="4">
         <v>0</v>
       </c>
+      <c r="O36" s="9" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:15">
       <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="5">
-        <v>42161</v>
+        <v>42162</v>
       </c>
       <c r="C37" s="8">
-        <v>0.43402777777777773</v>
+        <v>0.50486111111111109</v>
       </c>
       <c r="D37" s="8">
-        <v>0.63055555555555554</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G37" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H37" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I37" s="4">
         <v>0.01</v>
@@ -4879,10 +5139,10 @@
         <v>0</v>
       </c>
       <c r="K37" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L37" s="4">
-        <v>-2.8</v>
+        <v>5.2</v>
       </c>
       <c r="M37" s="4">
         <v>0</v>
@@ -4890,31 +5150,34 @@
       <c r="N37" s="4">
         <v>0</v>
       </c>
+      <c r="O37" s="9" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:15">
       <c r="A38" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="5">
-        <v>42161</v>
+        <v>42160</v>
       </c>
       <c r="C38" s="8">
-        <v>0.43402777777777773</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D38" s="8">
-        <v>0.63055555555555554</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G38" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H38" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I38" s="4">
         <v>0.01</v>
@@ -4923,10 +5186,10 @@
         <v>0</v>
       </c>
       <c r="K38" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L38" s="4">
-        <v>-0.4</v>
+        <v>-5.2</v>
       </c>
       <c r="M38" s="4">
         <v>0</v>
@@ -4934,8 +5197,11 @@
       <c r="N38" s="4">
         <v>0</v>
       </c>
+      <c r="O38" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:15">
       <c r="A39" s="4" t="s">
         <v>38</v>
       </c>
@@ -4943,22 +5209,22 @@
         <v>42161</v>
       </c>
       <c r="C39" s="8">
-        <v>0.43402777777777773</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D39" s="8">
-        <v>0.63055555555555554</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G39" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H39" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I39" s="4">
         <v>0.01</v>
@@ -4967,10 +5233,10 @@
         <v>0</v>
       </c>
       <c r="K39" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L39" s="4">
-        <v>0.4</v>
+        <v>-5.2</v>
       </c>
       <c r="M39" s="4">
         <v>0</v>
@@ -4978,8 +5244,11 @@
       <c r="N39" s="4">
         <v>0</v>
       </c>
+      <c r="O39" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:15">
       <c r="A40" s="4" t="s">
         <v>38</v>
       </c>
@@ -4993,10 +5262,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="G40" s="4">
         <v>1.49</v>
@@ -5011,36 +5280,39 @@
         <v>0</v>
       </c>
       <c r="K40" s="4">
+        <v>0</v>
+      </c>
+      <c r="L40" s="4">
         <v>0.4</v>
       </c>
-      <c r="L40" s="4">
-        <v>-2</v>
-      </c>
       <c r="M40" s="4">
         <v>0</v>
       </c>
       <c r="N40" s="4">
         <v>0</v>
       </c>
+      <c r="O40" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:15">
       <c r="A41" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="5">
-        <v>42162</v>
+        <v>42160</v>
       </c>
       <c r="C41" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D41" s="8">
-        <v>0.83333333333333337</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G41" s="4">
         <v>1.49</v>
@@ -5055,36 +5327,39 @@
         <v>0</v>
       </c>
       <c r="K41" s="4">
+        <v>0</v>
+      </c>
+      <c r="L41" s="4">
         <v>0.4</v>
       </c>
-      <c r="L41" s="4">
-        <v>-3.6</v>
-      </c>
       <c r="M41" s="4">
         <v>0</v>
       </c>
       <c r="N41" s="4">
         <v>0</v>
       </c>
+      <c r="O41" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:15">
       <c r="A42" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B42" s="5">
-        <v>42162</v>
+        <v>42161</v>
       </c>
       <c r="C42" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D42" s="8">
-        <v>0.83333333333333337</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G42" s="4">
         <v>1.49</v>
@@ -5099,19 +5374,22 @@
         <v>0</v>
       </c>
       <c r="K42" s="4">
+        <v>0</v>
+      </c>
+      <c r="L42" s="4">
         <v>0.4</v>
       </c>
-      <c r="L42" s="4">
-        <v>2</v>
-      </c>
       <c r="M42" s="4">
         <v>0</v>
       </c>
       <c r="N42" s="4">
         <v>0</v>
       </c>
+      <c r="O42" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:15">
       <c r="A43" s="4" t="s">
         <v>38</v>
       </c>
@@ -5125,10 +5403,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G43" s="4">
         <v>1.49</v>
@@ -5143,10 +5421,10 @@
         <v>0</v>
       </c>
       <c r="K43" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L43" s="4">
-        <v>0</v>
+        <v>-5.2</v>
       </c>
       <c r="M43" s="4">
         <v>0</v>
@@ -5154,19 +5432,22 @@
       <c r="N43" s="4">
         <v>0</v>
       </c>
+      <c r="O43" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:15">
       <c r="A44" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B44" s="5">
-        <v>42162</v>
+        <v>42160</v>
       </c>
       <c r="C44" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D44" s="8">
-        <v>0.83333333333333337</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>31</v>
@@ -5190,7 +5471,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="4">
-        <v>-4.4000000000000004</v>
+        <v>1.2</v>
       </c>
       <c r="M44" s="4">
         <v>0</v>
@@ -5198,25 +5479,28 @@
       <c r="N44" s="4">
         <v>0</v>
       </c>
+      <c r="O44" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:15">
       <c r="A45" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="5">
-        <v>42162</v>
+        <v>42161</v>
       </c>
       <c r="C45" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D45" s="8">
-        <v>0.83333333333333337</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G45" s="4">
         <v>1.49</v>
@@ -5234,7 +5518,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="4">
-        <v>-1.2</v>
+        <v>1.2</v>
       </c>
       <c r="M45" s="4">
         <v>0</v>
@@ -5242,8 +5526,11 @@
       <c r="N45" s="4">
         <v>0</v>
       </c>
+      <c r="O45" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:15">
       <c r="A46" s="4" t="s">
         <v>38</v>
       </c>
@@ -5260,7 +5547,7 @@
         <v>31</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G46" s="4">
         <v>1.49</v>
@@ -5278,7 +5565,7 @@
         <v>0</v>
       </c>
       <c r="L46" s="4">
-        <v>1.2</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="M46" s="4">
         <v>0</v>
@@ -5286,25 +5573,28 @@
       <c r="N46" s="4">
         <v>0</v>
       </c>
+      <c r="O46" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:15">
       <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B47" s="5">
-        <v>42162</v>
+        <v>42160</v>
       </c>
       <c r="C47" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D47" s="8">
-        <v>0.83333333333333337</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G47" s="4">
         <v>1.49</v>
@@ -5330,25 +5620,28 @@
       <c r="N47" s="4">
         <v>0</v>
       </c>
+      <c r="O47" s="9" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:15">
       <c r="A48" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B48" s="5">
-        <v>42162</v>
+        <v>42161</v>
       </c>
       <c r="C48" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D48" s="8">
-        <v>0.83333333333333337</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="G48" s="4">
         <v>1.49</v>
@@ -5366,7 +5659,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="4">
-        <v>2.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="M48" s="4">
         <v>0</v>
@@ -5374,8 +5667,11 @@
       <c r="N48" s="4">
         <v>0</v>
       </c>
+      <c r="O48" s="9" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:15">
       <c r="A49" s="4" t="s">
         <v>38</v>
       </c>
@@ -5389,10 +5685,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="G49" s="4">
         <v>1.49</v>
@@ -5410,7 +5706,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="4">
-        <v>-0.4</v>
+        <v>-1.2</v>
       </c>
       <c r="M49" s="4">
         <v>0</v>
@@ -5418,25 +5714,28 @@
       <c r="N49" s="4">
         <v>0</v>
       </c>
+      <c r="O49" s="9" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:15">
       <c r="A50" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B50" s="5">
-        <v>42162</v>
+        <v>42160</v>
       </c>
       <c r="C50" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D50" s="8">
-        <v>0.83333333333333337</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G50" s="4">
         <v>1.49</v>
@@ -5454,7 +5753,7 @@
         <v>0</v>
       </c>
       <c r="L50" s="4">
-        <v>-2.8</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="M50" s="4">
         <v>0</v>
@@ -5462,25 +5761,28 @@
       <c r="N50" s="4">
         <v>0</v>
       </c>
+      <c r="O50" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:15">
       <c r="A51" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B51" s="5">
-        <v>42162</v>
+        <v>42161</v>
       </c>
       <c r="C51" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D51" s="8">
-        <v>0.83333333333333337</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G51" s="4">
         <v>1.49</v>
@@ -5498,7 +5800,7 @@
         <v>0</v>
       </c>
       <c r="L51" s="4">
-        <v>5.2</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="M51" s="4">
         <v>0</v>
@@ -5506,8 +5808,11 @@
       <c r="N51" s="4">
         <v>0</v>
       </c>
+      <c r="O51" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:15">
       <c r="A52" s="4" t="s">
         <v>38</v>
       </c>
@@ -5521,10 +5826,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G52" s="4">
         <v>1.49</v>
@@ -5542,7 +5847,7 @@
         <v>0</v>
       </c>
       <c r="L52" s="4">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
       <c r="M52" s="4">
         <v>0</v>
@@ -5550,25 +5855,28 @@
       <c r="N52" s="4">
         <v>0</v>
       </c>
+      <c r="O52" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:15">
       <c r="A53" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B53" s="5">
-        <v>42162</v>
+        <v>42160</v>
       </c>
       <c r="C53" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D53" s="8">
-        <v>0.83333333333333337</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="G53" s="4">
         <v>1.49</v>
@@ -5586,7 +5894,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="4">
-        <v>-5.2</v>
+        <v>-1.2</v>
       </c>
       <c r="M53" s="4">
         <v>0</v>
@@ -5594,31 +5902,34 @@
       <c r="N53" s="4">
         <v>0</v>
       </c>
+      <c r="O53" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:15">
       <c r="A54" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B54" s="5">
-        <v>42162</v>
+        <v>42161</v>
       </c>
       <c r="C54" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D54" s="8">
-        <v>0.69791666666666663</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G54" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H54" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I54" s="4">
         <v>0.01</v>
@@ -5627,10 +5938,10 @@
         <v>0</v>
       </c>
       <c r="K54" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L54" s="4">
-        <v>0.4</v>
+        <v>-1.2</v>
       </c>
       <c r="M54" s="4">
         <v>0</v>
@@ -5638,8 +5949,11 @@
       <c r="N54" s="4">
         <v>0</v>
       </c>
+      <c r="O54" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:15">
       <c r="A55" s="4" t="s">
         <v>38</v>
       </c>
@@ -5650,19 +5964,19 @@
         <v>0.50486111111111109</v>
       </c>
       <c r="D55" s="8">
-        <v>0.69791666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G55" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H55" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I55" s="4">
         <v>0.01</v>
@@ -5671,10 +5985,10 @@
         <v>0</v>
       </c>
       <c r="K55" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L55" s="4">
-        <v>-0.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="M55" s="4">
         <v>0</v>
@@ -5682,31 +5996,34 @@
       <c r="N55" s="4">
         <v>0</v>
       </c>
+      <c r="O55" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:15">
       <c r="A56" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B56" s="5">
-        <v>42162</v>
+        <v>42160</v>
       </c>
       <c r="C56" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.71388888888888891</v>
       </c>
       <c r="D56" s="8">
-        <v>0.69791666666666663</v>
+        <v>0.73472222222222217</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G56" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H56" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I56" s="4">
         <v>0.01</v>
@@ -5715,10 +6032,10 @@
         <v>0</v>
       </c>
       <c r="K56" s="4">
-        <v>0.75</v>
+        <v>3</v>
       </c>
       <c r="L56" s="4">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="M56" s="4">
         <v>0</v>
@@ -5726,31 +6043,34 @@
       <c r="N56" s="4">
         <v>0</v>
       </c>
+      <c r="O56" s="9" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:15">
       <c r="A57" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B57" s="5">
-        <v>42162</v>
+        <v>42161</v>
       </c>
       <c r="C57" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D57" s="8">
-        <v>0.69791666666666663</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="G57" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H57" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I57" s="4">
         <v>0.01</v>
@@ -5759,10 +6079,10 @@
         <v>0</v>
       </c>
       <c r="K57" s="4">
-        <v>0.75</v>
+        <v>3</v>
       </c>
       <c r="L57" s="4">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="M57" s="4">
         <v>0</v>
@@ -5770,8 +6090,11 @@
       <c r="N57" s="4">
         <v>0</v>
       </c>
+      <c r="O57" s="9" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:15">
       <c r="A58" s="4" t="s">
         <v>38</v>
       </c>
@@ -5782,19 +6105,19 @@
         <v>0.50486111111111109</v>
       </c>
       <c r="D58" s="8">
-        <v>0.69791666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="G58" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="H58" s="4">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="I58" s="4">
         <v>0.01</v>
@@ -5803,24 +6126,27 @@
         <v>0</v>
       </c>
       <c r="K58" s="4">
-        <v>0.75</v>
+        <v>3</v>
       </c>
       <c r="L58" s="4">
-        <v>-2.8</v>
+        <v>0</v>
       </c>
       <c r="M58" s="4">
         <v>0</v>
       </c>
       <c r="N58" s="4">
         <v>0</v>
+      </c>
+      <c r="O58" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:O476">
-    <sortCondition descending="1" ref="B2:B476"/>
-    <sortCondition ref="E2:E476"/>
-    <sortCondition ref="C2:C476"/>
-    <sortCondition ref="F2:F476"/>
+  <sortState ref="A2:O58">
+    <sortCondition ref="E2:E58"/>
+    <sortCondition ref="F2:F58"/>
+    <sortCondition ref="B2:B58"/>
+    <sortCondition ref="C2:C58"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>